<commit_message>
TicketBulkUpdateTest Added to prod MW Config update in excel and Test msisdn updated
</commit_message>
<xml_diff>
--- a/resources/excels/MW.xlsx
+++ b/resources/excels/MW.xlsx
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'NFTRTickets-Reg'!$A$1:$AB$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'NFTRTickets-San'!$A$1:$AB$73</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3035,15 +3035,6 @@
     <t>Period</t>
   </si>
   <si>
-    <t>Charges (MK)</t>
-  </si>
-  <si>
-    <t>Bundle Price (MK)</t>
-  </si>
-  <si>
-    <t>Loan Amount (MK)</t>
-  </si>
-  <si>
     <t>Accumulator</t>
   </si>
   <si>
@@ -3143,242 +3134,251 @@
     <t>BenefitVoice|Data|SMS</t>
   </si>
   <si>
+    <t>Prod Customer Number</t>
+  </si>
+  <si>
+    <t>Prod SIM Number</t>
+  </si>
+  <si>
+    <t>QXByQDIwMjE</t>
+  </si>
+  <si>
+    <t>UmFvQDA4OTE</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>U29hQDIwMjE</t>
+  </si>
+  <si>
+    <t>89265029100300150859</t>
+  </si>
+  <si>
+    <t>Prod-Customer Number</t>
+  </si>
+  <si>
+    <t>Auth Pop up(TRUE/FALSE)</t>
+  </si>
+  <si>
+    <t>Voucher Id</t>
+  </si>
+  <si>
+    <t>reverseTransaction</t>
+  </si>
+  <si>
+    <t>resetPin</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>unblock</t>
+  </si>
+  <si>
+    <t>sendNotification</t>
+  </si>
+  <si>
+    <t>voucher</t>
+  </si>
+  <si>
+    <t>resetMe2UPassword</t>
+  </si>
+  <si>
+    <t>simUnBarring</t>
+  </si>
+  <si>
+    <t>simBarring</t>
+  </si>
+  <si>
+    <t>changeServiceClass</t>
+  </si>
+  <si>
+    <t>Question Label</t>
+  </si>
+  <si>
+    <t>Question_Key</t>
+  </si>
+  <si>
+    <t>Answer_key</t>
+  </si>
+  <si>
+    <t>Airtel Money Name</t>
+  </si>
+  <si>
+    <t>AM_NAME</t>
+  </si>
+  <si>
+    <t>cs-am-service/v1/profile.result.firstName</t>
+  </si>
+  <si>
+    <t>Available Credit Balance</t>
+  </si>
+  <si>
+    <t>AVAILABLE_CREDIT_BALANCE</t>
+  </si>
+  <si>
+    <t>cs-gsm-service/v1/account/plans.result.mainAccountBalance.balance</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>cs-gsm-service/v1/gsm/kyc.result.dob</t>
+  </si>
+  <si>
+    <t>GSM Name</t>
+  </si>
+  <si>
+    <t>GSM_NAME</t>
+  </si>
+  <si>
+    <t>cs-gsm-service/v1/gsm/kyc.result.name</t>
+  </si>
+  <si>
+    <t>Usage History Last Five Transaction</t>
+  </si>
+  <si>
+    <t>LAST_FIVE_TRANSACTIONS</t>
+  </si>
+  <si>
+    <t>Last Recharge Date</t>
+  </si>
+  <si>
+    <t>LAST_RECHARGE_DATE</t>
+  </si>
+  <si>
+    <t>cs-gsm-service/v1/recharge/history.result[0].dateTime</t>
+  </si>
+  <si>
+    <t>Last Recharge Value</t>
+  </si>
+  <si>
+    <t>LAST_RECHARGE_VALUE</t>
+  </si>
+  <si>
+    <t>cs-gsm-service/v1/recharge/history.result[0].charges</t>
+  </si>
+  <si>
+    <t>Last Transaction Amount</t>
+  </si>
+  <si>
+    <t>LAST_TRANSACTION_AMOUNT</t>
+  </si>
+  <si>
+    <t>cs-am-service/v1/transaction/history.result.data[0].amount</t>
+  </si>
+  <si>
+    <t>Last Transaction Id</t>
+  </si>
+  <si>
+    <t>LAST_TRANSACTION_ID</t>
+  </si>
+  <si>
+    <t>cs-am-service/v1/transaction/history.result.data[0].transactionId</t>
+  </si>
+  <si>
+    <t>Last Transaction Msisdn</t>
+  </si>
+  <si>
+    <t>LAST_TRANSACTION_MSISDN</t>
+  </si>
+  <si>
+    <t>cs-am-service/v1/transaction/history.result.data[0].msisdn</t>
+  </si>
+  <si>
+    <t>National Id</t>
+  </si>
+  <si>
+    <t>NATIONAL_ID</t>
+  </si>
+  <si>
+    <t>cs-gsm-service/v1/gsm/kyc.result.identificationNo</t>
+  </si>
+  <si>
+    <t>Register Id</t>
+  </si>
+  <si>
+    <t>REGISTERED_ID</t>
+  </si>
+  <si>
+    <t>Two Last Dialled Number</t>
+  </si>
+  <si>
+    <t>TWO_LAST_DIALLED_NUMBER</t>
+  </si>
+  <si>
+    <t>AM Wallet Balance</t>
+  </si>
+  <si>
+    <t>WALLET_BALANCE</t>
+  </si>
+  <si>
+    <t>cs-am-service/v1/profile.result.wallet[0].balance</t>
+  </si>
+  <si>
+    <t>210621000474</t>
+  </si>
+  <si>
+    <t>UC-UT Offer</t>
+  </si>
+  <si>
+    <t>Offer ID</t>
+  </si>
+  <si>
+    <t>Offer Name</t>
+  </si>
+  <si>
+    <t>Product ID</t>
+  </si>
+  <si>
+    <t>PAM Service ID</t>
+  </si>
+  <si>
+    <t>Offer Type</t>
+  </si>
+  <si>
+    <t>Offer State</t>
+  </si>
+  <si>
+    <t>No. Of DAs</t>
+  </si>
+  <si>
+    <t>Friends and Family</t>
+  </si>
+  <si>
+    <t>FnF Number</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>FnF Indicator</t>
+  </si>
+  <si>
+    <t>Charges (MWK)</t>
+  </si>
+  <si>
+    <t>Bundle Price (MWK)</t>
+  </si>
+  <si>
+    <t>Loan Amount (MWK)</t>
+  </si>
+  <si>
     <t>Amount
-(MK)</t>
+(MWK)</t>
   </si>
   <si>
     <t>Service Charge
-(MK)</t>
+(MWK)</t>
   </si>
   <si>
     <t>Pre balance
-(MK)</t>
+(MWK)</t>
   </si>
   <si>
     <t>Post balance
-(MK)</t>
-  </si>
-  <si>
-    <t>Prod Customer Number</t>
-  </si>
-  <si>
-    <t>Prod SIM Number</t>
-  </si>
-  <si>
-    <t>QXByQDIwMjE</t>
-  </si>
-  <si>
-    <t>UmFvQDA4OTE</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>U29hQDIwMjE</t>
-  </si>
-  <si>
-    <t>89265029100300150859</t>
-  </si>
-  <si>
-    <t>Prod-Customer Number</t>
-  </si>
-  <si>
-    <t>Auth Pop up(TRUE/FALSE)</t>
-  </si>
-  <si>
-    <t>Voucher Id</t>
-  </si>
-  <si>
-    <t>reverseTransaction</t>
-  </si>
-  <si>
-    <t>resetPin</t>
-  </si>
-  <si>
-    <t>block</t>
-  </si>
-  <si>
-    <t>unblock</t>
-  </si>
-  <si>
-    <t>sendNotification</t>
-  </si>
-  <si>
-    <t>voucher</t>
-  </si>
-  <si>
-    <t>resetMe2UPassword</t>
-  </si>
-  <si>
-    <t>simUnBarring</t>
-  </si>
-  <si>
-    <t>simBarring</t>
-  </si>
-  <si>
-    <t>changeServiceClass</t>
-  </si>
-  <si>
-    <t>Question Label</t>
-  </si>
-  <si>
-    <t>Question_Key</t>
-  </si>
-  <si>
-    <t>Answer_key</t>
-  </si>
-  <si>
-    <t>Airtel Money Name</t>
-  </si>
-  <si>
-    <t>AM_NAME</t>
-  </si>
-  <si>
-    <t>cs-am-service/v1/profile.result.firstName</t>
-  </si>
-  <si>
-    <t>Available Credit Balance</t>
-  </si>
-  <si>
-    <t>AVAILABLE_CREDIT_BALANCE</t>
-  </si>
-  <si>
-    <t>cs-gsm-service/v1/account/plans.result.mainAccountBalance.balance</t>
-  </si>
-  <si>
-    <t>DOB</t>
-  </si>
-  <si>
-    <t>cs-gsm-service/v1/gsm/kyc.result.dob</t>
-  </si>
-  <si>
-    <t>GSM Name</t>
-  </si>
-  <si>
-    <t>GSM_NAME</t>
-  </si>
-  <si>
-    <t>cs-gsm-service/v1/gsm/kyc.result.name</t>
-  </si>
-  <si>
-    <t>Usage History Last Five Transaction</t>
-  </si>
-  <si>
-    <t>LAST_FIVE_TRANSACTIONS</t>
-  </si>
-  <si>
-    <t>Last Recharge Date</t>
-  </si>
-  <si>
-    <t>LAST_RECHARGE_DATE</t>
-  </si>
-  <si>
-    <t>cs-gsm-service/v1/recharge/history.result[0].dateTime</t>
-  </si>
-  <si>
-    <t>Last Recharge Value</t>
-  </si>
-  <si>
-    <t>LAST_RECHARGE_VALUE</t>
-  </si>
-  <si>
-    <t>cs-gsm-service/v1/recharge/history.result[0].charges</t>
-  </si>
-  <si>
-    <t>Last Transaction Amount</t>
-  </si>
-  <si>
-    <t>LAST_TRANSACTION_AMOUNT</t>
-  </si>
-  <si>
-    <t>cs-am-service/v1/transaction/history.result.data[0].amount</t>
-  </si>
-  <si>
-    <t>Last Transaction Id</t>
-  </si>
-  <si>
-    <t>LAST_TRANSACTION_ID</t>
-  </si>
-  <si>
-    <t>cs-am-service/v1/transaction/history.result.data[0].transactionId</t>
-  </si>
-  <si>
-    <t>Last Transaction Msisdn</t>
-  </si>
-  <si>
-    <t>LAST_TRANSACTION_MSISDN</t>
-  </si>
-  <si>
-    <t>cs-am-service/v1/transaction/history.result.data[0].msisdn</t>
-  </si>
-  <si>
-    <t>National Id</t>
-  </si>
-  <si>
-    <t>NATIONAL_ID</t>
-  </si>
-  <si>
-    <t>cs-gsm-service/v1/gsm/kyc.result.identificationNo</t>
-  </si>
-  <si>
-    <t>Register Id</t>
-  </si>
-  <si>
-    <t>REGISTERED_ID</t>
-  </si>
-  <si>
-    <t>Two Last Dialled Number</t>
-  </si>
-  <si>
-    <t>TWO_LAST_DIALLED_NUMBER</t>
-  </si>
-  <si>
-    <t>AM Wallet Balance</t>
-  </si>
-  <si>
-    <t>WALLET_BALANCE</t>
-  </si>
-  <si>
-    <t>cs-am-service/v1/profile.result.wallet[0].balance</t>
-  </si>
-  <si>
-    <t>210621000474</t>
-  </si>
-  <si>
-    <t>UC-UT Offer</t>
-  </si>
-  <si>
-    <t>Offer ID</t>
-  </si>
-  <si>
-    <t>Offer Name</t>
-  </si>
-  <si>
-    <t>Product ID</t>
-  </si>
-  <si>
-    <t>PAM Service ID</t>
-  </si>
-  <si>
-    <t>Offer Type</t>
-  </si>
-  <si>
-    <t>Offer State</t>
-  </si>
-  <si>
-    <t>No. Of DAs</t>
-  </si>
-  <si>
-    <t>Friends and Family</t>
-  </si>
-  <si>
-    <t>FnF Number</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>FnF Indicator</t>
+(MWK)</t>
   </si>
 </sst>
 </file>
@@ -3731,7 +3731,7 @@
         <xdr:cNvPr id="2" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3779,7 +3779,7 @@
         <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3827,7 +3827,7 @@
         <xdr:cNvPr id="4" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3875,7 +3875,7 @@
         <xdr:cNvPr id="5" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4268,10 +4268,10 @@
         <v>217</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>1035</v>
+        <v>1028</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>1036</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -4279,7 +4279,7 @@
         <v>2390495</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="C2" t="s">
         <v>67</v>
@@ -4300,7 +4300,7 @@
         <v>78</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>1041</v>
+        <v>1034</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
@@ -4332,7 +4332,7 @@
         <v>2388192</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1037</v>
+        <v>1030</v>
       </c>
       <c r="C3" t="s">
         <v>66</v>
@@ -4349,7 +4349,7 @@
         <v>2390495</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="C4" t="s">
         <v>175</v>
@@ -4369,7 +4369,7 @@
         <v>2394650</v>
       </c>
       <c r="B5" t="s">
-        <v>1040</v>
+        <v>1033</v>
       </c>
       <c r="C5" t="s">
         <v>215</v>
@@ -4389,10 +4389,10 @@
         <v>13221514</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>1038</v>
+        <v>1031</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>1039</v>
+        <v>1032</v>
       </c>
       <c r="D6" s="42">
         <v>998270828</v>
@@ -4631,7 +4631,7 @@
         <v>56</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>1042</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -5019,13 +5019,13 @@
         <v>851</v>
       </c>
       <c r="H1" s="44" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>1043</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5050,7 +5050,7 @@
     </row>
     <row r="3" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>1044</v>
+        <v>1037</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -5059,10 +5059,10 @@
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
       <c r="H3" s="38" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="J3" s="38" t="b">
         <v>0</v>
@@ -5070,7 +5070,7 @@
     </row>
     <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>1045</v>
+        <v>1038</v>
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
@@ -5086,7 +5086,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>1046</v>
+        <v>1039</v>
       </c>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -5102,7 +5102,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>1047</v>
+        <v>1040</v>
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
@@ -5118,7 +5118,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>1048</v>
+        <v>1041</v>
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -5134,7 +5134,7 @@
     </row>
     <row r="8" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>1049</v>
+        <v>1042</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
@@ -5150,7 +5150,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>1050</v>
+        <v>1043</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
@@ -5166,7 +5166,7 @@
     </row>
     <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>1051</v>
+        <v>1044</v>
       </c>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
@@ -5182,7 +5182,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>1052</v>
+        <v>1045</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -5198,7 +5198,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>1053</v>
+        <v>1046</v>
       </c>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
@@ -5214,7 +5214,7 @@
     </row>
     <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>1054</v>
+        <v>1047</v>
       </c>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
@@ -5252,35 +5252,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>1055</v>
+        <v>1048</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>1056</v>
+        <v>1049</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>1057</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>1058</v>
+        <v>1051</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1059</v>
+        <v>1052</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>1060</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
-        <v>1061</v>
+        <v>1054</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1062</v>
+        <v>1055</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>1063</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -5288,125 +5288,125 @@
         <v>160</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1064</v>
+        <v>1057</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>1065</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>1066</v>
+        <v>1059</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>1067</v>
+        <v>1060</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>1068</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>1069</v>
+        <v>1062</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>1070</v>
+        <v>1063</v>
       </c>
       <c r="C6" s="46"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>1071</v>
+        <v>1064</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>1072</v>
+        <v>1065</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>1073</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>1074</v>
+        <v>1067</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>1075</v>
+        <v>1068</v>
       </c>
       <c r="C8" s="38" t="s">
-        <v>1076</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>1077</v>
+        <v>1070</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>1078</v>
+        <v>1071</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>1079</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>1080</v>
+        <v>1073</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>1081</v>
+        <v>1074</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>1082</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>1083</v>
+        <v>1076</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>1084</v>
+        <v>1077</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>1085</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
-        <v>1086</v>
+        <v>1079</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>1087</v>
+        <v>1080</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>1088</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>1089</v>
+        <v>1082</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>1090</v>
+        <v>1083</v>
       </c>
       <c r="C13" s="46"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>1091</v>
+        <v>1084</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>1092</v>
+        <v>1085</v>
       </c>
       <c r="C14" s="46"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>1093</v>
+        <v>1086</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>1094</v>
+        <v>1087</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>1095</v>
+        <v>1088</v>
       </c>
     </row>
   </sheetData>
@@ -5557,7 +5557,7 @@
         <v>823</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5656,8 +5656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5702,16 +5702,16 @@
         <v>186</v>
       </c>
       <c r="J1" s="37" t="s">
+        <v>1022</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>1023</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>1025</v>
-      </c>
-      <c r="K1" s="37" t="s">
-        <v>1026</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1027</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>1028</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5719,7 +5719,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>187</v>
@@ -5773,7 +5773,7 @@
         <v>194</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>995</v>
+        <v>1102</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>192</v>
@@ -5782,7 +5782,7 @@
         <v>195</v>
       </c>
       <c r="E4" s="38" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>189</v>
@@ -5821,7 +5821,7 @@
         <v>201</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>996</v>
+        <v>1103</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -5940,7 +5940,7 @@
         <v>886</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>997</v>
+        <v>1104</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>887</v>
@@ -6047,7 +6047,7 @@
         <v>983</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>995</v>
+        <v>1102</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>192</v>
@@ -6137,19 +6137,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
+        <v>995</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>996</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>997</v>
+      </c>
+      <c r="D17" s="37" t="s">
         <v>998</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="E17" s="37" t="s">
         <v>999</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>1000</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>1001</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>1002</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -6162,19 +6162,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D18" s="37" t="s">
         <v>1008</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="E18" s="37" t="s">
         <v>1009</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>1010</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>1011</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>1012</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>845</v>
@@ -6189,66 +6189,66 @@
     </row>
     <row r="19" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>1031</v>
+        <v>1105</v>
       </c>
       <c r="C19" s="37" t="s">
         <v>161</v>
       </c>
       <c r="D19" s="37" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>1013</v>
+      </c>
+      <c r="G19" s="37" t="s">
         <v>1014</v>
-      </c>
-      <c r="E19" s="37" t="s">
-        <v>1015</v>
-      </c>
-      <c r="F19" s="37" t="s">
-        <v>1016</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>1017</v>
       </c>
       <c r="H19" s="37" t="s">
         <v>188</v>
       </c>
       <c r="I19" s="40" t="s">
-        <v>1032</v>
+        <v>1106</v>
       </c>
       <c r="J19" s="40" t="s">
-        <v>1033</v>
+        <v>1107</v>
       </c>
       <c r="K19" s="40" t="s">
-        <v>1034</v>
+        <v>1108</v>
       </c>
       <c r="L19" s="37" t="s">
         <v>189</v>
       </c>
       <c r="M19" s="37" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>192</v>
       </c>
       <c r="D20" s="37" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G20" s="37" t="s">
         <v>1021</v>
-      </c>
-      <c r="E20" s="37" t="s">
-        <v>1022</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>1023</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>1024</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -6259,34 +6259,34 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>1097</v>
+        <v>1090</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1098</v>
+        <v>1091</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>1099</v>
+        <v>1092</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>1100</v>
+        <v>1093</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>214</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>1101</v>
+        <v>1094</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>1102</v>
+        <v>1095</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>1103</v>
+        <v>1096</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>1104</v>
+        <v>1097</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -6294,22 +6294,22 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>1105</v>
+        <v>1098</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1106</v>
+        <v>1099</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1107</v>
+        <v>1100</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>214</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>1108</v>
+        <v>1101</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>845</v>
@@ -11635,7 +11635,7 @@
         <v>140</v>
       </c>
       <c r="BG2" t="s">
-        <v>1096</v>
+        <v>1089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>